<commit_message>
Add hypothetical "exceptional tree" to View Ave numbers
</commit_message>
<xml_diff>
--- a/8 View Ave/8 View Ave.xlsx
+++ b/8 View Ave/8 View Ave.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kent/Dev/Noho/8 View Ave/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6163F40-CA51-9843-9F29-7747A2155915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F617BF69-F886-DA45-8A1B-DF2601914612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="1340" windowWidth="25320" windowHeight="12520" xr2:uid="{C1FB6AE6-6796-3044-8B24-CA96EBAEC7BC}"/>
+    <workbookView xWindow="4080" yWindow="1340" windowWidth="25320" windowHeight="12520" xr2:uid="{C1FB6AE6-6796-3044-8B24-CA96EBAEC7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Northeast - 1 tree</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Non-canopy</t>
+  </si>
+  <si>
+    <t>With exceptional bonus</t>
   </si>
 </sst>
 </file>
@@ -522,398 +525,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D4F6D-4B75-ED44-B535-E57A547B4367}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <f>IF(A3&gt;=30, A3*1.5, A3)</f>
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>13</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <f>F3*G3</f>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f>G3*H3</f>
         <v>26</v>
       </c>
-      <c r="J3">
-        <f>F3*H3</f>
+      <c r="K3">
+        <f>G3*I3</f>
         <v>26</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>30</v>
       </c>
-      <c r="M3">
-        <f>IF(K3="Y", J3, 0)</f>
+      <c r="N3">
+        <f>IF(L3="Y", K3, 0)</f>
         <v>0</v>
       </c>
-      <c r="N3">
-        <f>IF(K3="N", J3, 0)</f>
+      <c r="O3">
+        <f>IF(L3="N", K3, 0)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" ref="C4:C41" si="0">IF(A4&gt;=30, A4*1.5, A4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
       <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2.5</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I9" si="0">F4*G4</f>
+      <c r="J4">
+        <f t="shared" ref="J4:J9" si="1">G4*H4</f>
         <v>6</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J9" si="1">F4*H4</f>
+      <c r="K4">
+        <f t="shared" ref="K4:K9" si="2">G4*I4</f>
         <v>7.5</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>35</v>
       </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M9" si="2">IF(K4="Y", J4, 0)</f>
+      <c r="N4">
+        <f t="shared" ref="N4:N9" si="3">IF(L4="Y", K4, 0)</f>
         <v>0</v>
       </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N9" si="3">IF(K4="N", J4, 0)</f>
+      <c r="O4">
+        <f t="shared" ref="O4:O9" si="4">IF(L4="N", K4, 0)</f>
         <v>7.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
       <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2.5</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>33</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6">
-        <v>82</v>
-      </c>
-      <c r="M6">
+      <c r="K6">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6">
+        <v>82</v>
+      </c>
       <c r="N6">
         <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
         <v>33</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>131</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="2"/>
-        <v>3</v>
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>25</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2.5</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>50</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>62.5</v>
-      </c>
-      <c r="K8" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8">
         <v>50</v>
       </c>
-      <c r="M8">
+      <c r="K8">
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8">
+        <v>50</v>
+      </c>
       <c r="N8">
         <f t="shared" si="3"/>
+        <v>62.5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
       <c r="H9">
         <v>3</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
         <v>33</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>100</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>3</v>
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>46.5</v>
+      </c>
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="F10">
-        <f>SUM(F3:F9)</f>
+      <c r="G10">
+        <f>SUM(G3:G9)</f>
         <v>48</v>
-      </c>
-      <c r="I10">
-        <f>SUM(I3:I9)</f>
-        <v>100</v>
       </c>
       <c r="J10">
         <f>SUM(J3:J9)</f>
+        <v>100</v>
+      </c>
+      <c r="K10">
+        <f>SUM(K3:K9)</f>
         <v>115.5</v>
-      </c>
-      <c r="M10">
-        <f>SUM(M3:M9)</f>
-        <v>74.5</v>
       </c>
       <c r="N10">
         <f>SUM(N3:N9)</f>
+        <v>74.5</v>
+      </c>
+      <c r="O10">
+        <f>SUM(O3:O9)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>38</v>
       </c>
@@ -921,48 +966,86 @@
         <f>SUM(A6:A13)</f>
         <v>211</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -970,28 +1053,50 @@
         <f>SUM(A16:A23)</f>
         <v>219</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>30</v>
       </c>
@@ -999,38 +1104,68 @@
         <f>SUM(A26:A29)</f>
         <v>104</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>21</v>
       </c>
@@ -1038,24 +1173,52 @@
         <f>SUM(A32:A37)</f>
         <v>145</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>36</v>
       </c>
       <c r="B41">
         <f>SUM(A40:A41)</f>
         <v>64</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <f>SUM(B3:B41)</f>
+        <v>777</v>
+      </c>
+      <c r="C42">
+        <f>SUM(C3:C41)</f>
+        <v>949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for latest View Ave plans (27 trees removed)
</commit_message>
<xml_diff>
--- a/8 View Ave/8 View Ave.xlsx
+++ b/8 View Ave/8 View Ave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kent/Dev/Noho/8 View Ave/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F617BF69-F886-DA45-8A1B-DF2601914612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B648124-C3E0-C346-B5F4-BCB61DEA6540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1340" windowWidth="25320" windowHeight="12520" xr2:uid="{C1FB6AE6-6796-3044-8B24-CA96EBAEC7BC}"/>
+    <workbookView xWindow="25840" yWindow="3400" windowWidth="21920" windowHeight="18900" xr2:uid="{C1FB6AE6-6796-3044-8B24-CA96EBAEC7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Northeast - 1 tree</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Six trees</t>
   </si>
   <si>
-    <t>SW two trees</t>
-  </si>
-  <si>
     <t>Trees removed</t>
   </si>
   <si>
@@ -147,6 +144,36 @@
   </si>
   <si>
     <t>With exceptional bonus</t>
+  </si>
+  <si>
+    <t>Chionanthus Virginicus</t>
+  </si>
+  <si>
+    <t>Fringetree</t>
+  </si>
+  <si>
+    <t>Cladastrus Kentukea</t>
+  </si>
+  <si>
+    <t>Yellowwood</t>
+  </si>
+  <si>
+    <t>Quercus Bicolor</t>
+  </si>
+  <si>
+    <t>Swamp White Oak</t>
+  </si>
+  <si>
+    <t>Oxydendron Arboreum</t>
+  </si>
+  <si>
+    <t>Sourwood</t>
+  </si>
+  <si>
+    <t>Canopy count</t>
+  </si>
+  <si>
+    <t>Non-canopy count</t>
   </si>
 </sst>
 </file>
@@ -525,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D4F6D-4B75-ED44-B535-E57A547B4367}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,59 +565,63 @@
     <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
       <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>34</v>
       </c>
@@ -602,13 +633,13 @@
         <v>51</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
       <c r="G3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -618,40 +649,44 @@
       </c>
       <c r="J3">
         <f>G3*H3</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K3">
         <f>G3*I3</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3">
         <v>30</v>
       </c>
       <c r="N3">
-        <f>IF(L3="Y", K3, 0)</f>
+        <f>IF(L3="Y", G3, 0)</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f>IF(L3="N", K3, 0)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f>IF(L3="Y", J3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>IF(L3="N", J3, 0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C4">
-        <f t="shared" ref="C4:C41" si="0">IF(A4&gt;=30, A4*1.5, A4)</f>
+        <f t="shared" ref="C4:C45" si="0">IF(A4&gt;=30, A4*1.5, A4)</f>
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -660,40 +695,44 @@
         <v>2.5</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J9" si="1">G4*H4</f>
-        <v>6</v>
+        <f t="shared" ref="J4:J13" si="1">G4*H4</f>
+        <v>8</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K9" si="2">G4*I4</f>
-        <v>7.5</v>
+        <f t="shared" ref="K4:K13" si="2">G4*I4</f>
+        <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4">
         <v>35</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N9" si="3">IF(L4="Y", K4, 0)</f>
+        <f t="shared" ref="N4:N13" si="3">IF(L4="Y", G4, 0)</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O9" si="4">IF(L4="N", K4, 0)</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O4:O13" si="4">IF(L4="Y", J4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P13" si="5">IF(L4="N", J4, 0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
       <c r="G5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -703,14 +742,14 @@
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>17.5</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5">
         <v>33</v>
@@ -721,45 +760,43 @@
       </c>
       <c r="O5">
         <f t="shared" si="4"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2.5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J7" si="6">G6*H6</f>
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K7" si="7">G6*I6</f>
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
         <v>32</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
       <c r="M6">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
@@ -767,357 +804,533 @@
       </c>
       <c r="O6">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>22</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>12.5</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M7">
-        <v>131</v>
+        <v>30</v>
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G8">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>62.5</v>
+        <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M8">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>62.5</v>
+        <v>4</v>
       </c>
       <c r="O8">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>23</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>12.5</v>
       </c>
       <c r="L9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M9">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10">
+        <v>131</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>2.5</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>62.5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11">
+        <v>50</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13">
+        <v>60</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>31</v>
       </c>
-      <c r="C10">
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>46.5</v>
       </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10">
-        <f>SUM(G3:G9)</f>
-        <v>48</v>
-      </c>
-      <c r="J10">
-        <f>SUM(J3:J9)</f>
-        <v>100</v>
-      </c>
-      <c r="K10">
-        <f>SUM(K3:K9)</f>
-        <v>115.5</v>
-      </c>
-      <c r="N10">
-        <f>SUM(N3:N9)</f>
-        <v>74.5</v>
-      </c>
-      <c r="O10">
-        <f>SUM(O3:O9)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14">
+        <f>SUM(G3:G13)</f>
+        <v>79</v>
+      </c>
+      <c r="J14">
+        <f>SUM(J3:J13)</f>
+        <v>171</v>
+      </c>
+      <c r="K14">
+        <f>SUM(K3:K13)</f>
+        <v>197</v>
+      </c>
+      <c r="N14">
+        <f>SUM(N3:N13)</f>
+        <v>44</v>
+      </c>
+      <c r="O14">
+        <f>SUM(O3:O13)</f>
+        <v>101</v>
+      </c>
+      <c r="P14">
+        <f>SUM(P3:P13)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>23</v>
       </c>
-      <c r="C11">
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="M15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15">
+        <f>G14-N14</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>20</v>
       </c>
-      <c r="C12">
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>38</v>
-      </c>
-      <c r="B13">
-        <f>SUM(A6:A13)</f>
-        <v>211</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>47</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>70.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <f>SUM(A8:A17)</f>
+        <v>211</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>23</v>
-      </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>20</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="A19" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23">
-        <f>SUM(A16:A23)</f>
-        <v>219</v>
-      </c>
       <c r="C23">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>29</v>
+      </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>3</v>
+      <c r="A25" s="1">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <f>SUM(A20:A27)</f>
+        <v>219</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>31</v>
       </c>
-      <c r="C27">
+      <c r="C31">
         <f t="shared" si="0"/>
         <v>46.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>20</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>30</v>
-      </c>
-      <c r="B29">
-        <f>SUM(A26:A29)</f>
-        <v>104</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1131,94 +1344,121 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <f>SUM(A30:A33)</f>
+        <v>104</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>35</v>
-      </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>21</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="A35" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
+        <v>26</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>21</v>
       </c>
-      <c r="B37">
-        <f>SUM(A32:A37)</f>
-        <v>145</v>
-      </c>
-      <c r="C37">
+      <c r="C39">
         <f t="shared" si="0"/>
         <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B41">
-        <f>SUM(A40:A41)</f>
-        <v>64</v>
+        <f>SUM(A36:A41)</f>
+        <v>145</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42">
-        <f>SUM(B3:B41)</f>
-        <v>777</v>
-      </c>
       <c r="C42">
-        <f>SUM(C3:C41)</f>
-        <v>949</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45">
+        <f>SUM(A44:A45)</f>
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <f>SUM(B3:B45)</f>
+        <v>713</v>
+      </c>
+      <c r="C46">
+        <f>SUM(C3:C45)</f>
+        <v>867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8 View Ave update
</commit_message>
<xml_diff>
--- a/8 View Ave/8 View Ave.xlsx
+++ b/8 View Ave/8 View Ave.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kent/Dev/Noho/8 View Ave/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B648124-C3E0-C346-B5F4-BCB61DEA6540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBF974B-B5E9-DF43-83EA-4A04666904F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25840" yWindow="3400" windowWidth="21920" windowHeight="18900" xr2:uid="{C1FB6AE6-6796-3044-8B24-CA96EBAEC7BC}"/>
+    <workbookView xWindow="19960" yWindow="2220" windowWidth="28300" windowHeight="19020" xr2:uid="{C1FB6AE6-6796-3044-8B24-CA96EBAEC7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Northeast - 1 tree</t>
   </si>
@@ -174,12 +174,33 @@
   </si>
   <si>
     <t>Non-canopy count</t>
+  </si>
+  <si>
+    <t>Replacement required</t>
+  </si>
+  <si>
+    <t>Trees planted</t>
+  </si>
+  <si>
+    <t>Mitigation required</t>
+  </si>
+  <si>
+    <t>Mitigation amount</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>With 100% Replacement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -215,9 +236,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,15 +576,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94D4F6D-4B75-ED44-B535-E57A547B4367}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" customWidth="1"/>
@@ -1204,7 +1226,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>38</v>
       </c>
@@ -1217,18 +1239,35 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <f>B46</f>
+        <v>713</v>
+      </c>
+      <c r="G19">
+        <f>B46</f>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>47</v>
       </c>
@@ -1236,8 +1275,19 @@
         <f t="shared" si="0"/>
         <v>70.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20">
+        <f>ROUND(F19/2, 0)</f>
+        <v>357</v>
+      </c>
+      <c r="G20">
+        <f>G19</f>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>29</v>
       </c>
@@ -1245,8 +1295,19 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21">
+        <f>J14</f>
+        <v>171</v>
+      </c>
+      <c r="G21">
+        <f>J14</f>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>23</v>
       </c>
@@ -1254,8 +1315,19 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22">
+        <f>F20-F21</f>
+        <v>186</v>
+      </c>
+      <c r="G22">
+        <f>G20-G21</f>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1263,8 +1335,19 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="2">
+        <f>F22*100</f>
+        <v>18600</v>
+      </c>
+      <c r="G23" s="2">
+        <f>G22*100</f>
+        <v>54200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>29</v>
       </c>
@@ -1273,7 +1356,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>30</v>
       </c>
@@ -1282,7 +1365,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>21</v>
       </c>
@@ -1291,7 +1374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -1304,18 +1387,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>23</v>
       </c>
@@ -1324,7 +1407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1333,7 +1416,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>20</v>
       </c>

</xml_diff>